<commit_message>
the deleting the unwanted files and creating saparate DDt tset class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/loginData.xlsx
+++ b/src/test/resources/TestData/loginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KoushikEclipsWorkspace\SecureBankDemoSelenium\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3A18F2-C64A-4C23-9552-4C6D5B58D512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7E651A-0E5B-4D8E-B5E5-7DE819C6EC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EBD6AFCA-C2A0-47C0-A4FC-5D694044A275}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>falied</t>
-  </si>
-  <si>
-    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -425,7 +422,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,9 +477,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="F7" s="1"/>

</xml_diff>